<commit_message>
Corrijo conflicto y sincronizo cambios
</commit_message>
<xml_diff>
--- a/proveedores.xlsx
+++ b/proveedores.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\portal-proveedores\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Pagina\portal-proveedores\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -685,9 +685,6 @@
     <t>0203ceuh</t>
   </si>
   <si>
-    <t>2063hqid</t>
-  </si>
-  <si>
     <t>9049yggk</t>
   </si>
   <si>
@@ -1046,6 +1043,9 @@
   </si>
   <si>
     <t>6820dsaa</t>
+  </si>
+  <si>
+    <t>5063hqid</t>
   </si>
 </sst>
 </file>
@@ -1391,8 +1391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1421,7 +1421,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>220</v>
+        <v>340</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1432,7 +1432,7 @@
         <v>54</v>
       </c>
       <c r="C3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1443,7 +1443,7 @@
         <v>207</v>
       </c>
       <c r="C4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1454,7 +1454,7 @@
         <v>132</v>
       </c>
       <c r="C5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1465,7 +1465,7 @@
         <v>108</v>
       </c>
       <c r="C6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1476,7 +1476,7 @@
         <v>90</v>
       </c>
       <c r="C7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1487,7 +1487,7 @@
         <v>152</v>
       </c>
       <c r="C8" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1509,7 +1509,7 @@
         <v>82</v>
       </c>
       <c r="C10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1520,7 +1520,7 @@
         <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1531,7 +1531,7 @@
         <v>120</v>
       </c>
       <c r="C12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1542,7 +1542,7 @@
         <v>122</v>
       </c>
       <c r="C13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1553,7 +1553,7 @@
         <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1564,7 +1564,7 @@
         <v>201</v>
       </c>
       <c r="C15" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1575,7 +1575,7 @@
         <v>92</v>
       </c>
       <c r="C16" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1586,7 +1586,7 @@
         <v>114</v>
       </c>
       <c r="C17" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1608,7 +1608,7 @@
         <v>88</v>
       </c>
       <c r="C19" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1619,7 +1619,7 @@
         <v>30</v>
       </c>
       <c r="C20" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1630,7 +1630,7 @@
         <v>128</v>
       </c>
       <c r="C21" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1641,7 +1641,7 @@
         <v>86</v>
       </c>
       <c r="C22" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1652,7 +1652,7 @@
         <v>142</v>
       </c>
       <c r="C23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1663,7 +1663,7 @@
         <v>96</v>
       </c>
       <c r="C24" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1674,7 +1674,7 @@
         <v>112</v>
       </c>
       <c r="C25" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -1685,7 +1685,7 @@
         <v>26</v>
       </c>
       <c r="C26" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1696,7 +1696,7 @@
         <v>76</v>
       </c>
       <c r="C27" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1707,7 +1707,7 @@
         <v>130</v>
       </c>
       <c r="C28" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1718,7 +1718,7 @@
         <v>179</v>
       </c>
       <c r="C29" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -1729,7 +1729,7 @@
         <v>36</v>
       </c>
       <c r="C30" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -1740,7 +1740,7 @@
         <v>191</v>
       </c>
       <c r="C31" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -1751,7 +1751,7 @@
         <v>209</v>
       </c>
       <c r="C32" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -1762,7 +1762,7 @@
         <v>20</v>
       </c>
       <c r="C33" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -1773,7 +1773,7 @@
         <v>62</v>
       </c>
       <c r="C34" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -1784,7 +1784,7 @@
         <v>94</v>
       </c>
       <c r="C35" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1795,7 +1795,7 @@
         <v>70</v>
       </c>
       <c r="C36" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -1806,7 +1806,7 @@
         <v>46</v>
       </c>
       <c r="C37" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -1817,7 +1817,7 @@
         <v>98</v>
       </c>
       <c r="C38" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -1828,7 +1828,7 @@
         <v>18</v>
       </c>
       <c r="C39" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -1839,7 +1839,7 @@
         <v>52</v>
       </c>
       <c r="C40" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -1850,7 +1850,7 @@
         <v>146</v>
       </c>
       <c r="C41" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -1861,7 +1861,7 @@
         <v>167</v>
       </c>
       <c r="C42" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1872,7 +1872,7 @@
         <v>110</v>
       </c>
       <c r="C43" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -1883,7 +1883,7 @@
         <v>169</v>
       </c>
       <c r="C44" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -1894,7 +1894,7 @@
         <v>144</v>
       </c>
       <c r="C45" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1905,7 +1905,7 @@
         <v>154</v>
       </c>
       <c r="C46" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -1916,7 +1916,7 @@
         <v>154</v>
       </c>
       <c r="C47" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1927,7 +1927,7 @@
         <v>48</v>
       </c>
       <c r="C48" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -1938,7 +1938,7 @@
         <v>56</v>
       </c>
       <c r="C49" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1949,7 +1949,7 @@
         <v>12</v>
       </c>
       <c r="C50" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1960,7 +1960,7 @@
         <v>66</v>
       </c>
       <c r="C51" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1971,7 +1971,7 @@
         <v>177</v>
       </c>
       <c r="C52" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1982,7 +1982,7 @@
         <v>148</v>
       </c>
       <c r="C53" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1993,7 +1993,7 @@
         <v>199</v>
       </c>
       <c r="C54" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -2004,7 +2004,7 @@
         <v>102</v>
       </c>
       <c r="C55" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -2015,7 +2015,7 @@
         <v>126</v>
       </c>
       <c r="C56" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -2026,7 +2026,7 @@
         <v>161</v>
       </c>
       <c r="C57" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -2037,7 +2037,7 @@
         <v>171</v>
       </c>
       <c r="C58" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -2048,7 +2048,7 @@
         <v>106</v>
       </c>
       <c r="C59" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -2059,7 +2059,7 @@
         <v>50</v>
       </c>
       <c r="C60" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -2070,7 +2070,7 @@
         <v>32</v>
       </c>
       <c r="C61" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -2081,7 +2081,7 @@
         <v>189</v>
       </c>
       <c r="C62" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -2092,7 +2092,7 @@
         <v>138</v>
       </c>
       <c r="C63" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -2103,7 +2103,7 @@
         <v>118</v>
       </c>
       <c r="C64" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -2114,7 +2114,7 @@
         <v>187</v>
       </c>
       <c r="C65" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -2125,7 +2125,7 @@
         <v>205</v>
       </c>
       <c r="C66" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -2136,7 +2136,7 @@
         <v>181</v>
       </c>
       <c r="C67" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -2147,7 +2147,7 @@
         <v>74</v>
       </c>
       <c r="C68" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
@@ -2158,7 +2158,7 @@
         <v>64</v>
       </c>
       <c r="C69" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -2169,7 +2169,7 @@
         <v>134</v>
       </c>
       <c r="C70" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -2180,7 +2180,7 @@
         <v>136</v>
       </c>
       <c r="C71" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -2191,7 +2191,7 @@
         <v>157</v>
       </c>
       <c r="C72" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -2202,7 +2202,7 @@
         <v>175</v>
       </c>
       <c r="C73" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -2213,7 +2213,7 @@
         <v>150</v>
       </c>
       <c r="C74" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -2224,7 +2224,7 @@
         <v>173</v>
       </c>
       <c r="C75" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -2235,7 +2235,7 @@
         <v>34</v>
       </c>
       <c r="C76" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -2246,7 +2246,7 @@
         <v>197</v>
       </c>
       <c r="C77" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -2257,7 +2257,7 @@
         <v>38</v>
       </c>
       <c r="C78" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -2279,7 +2279,7 @@
         <v>100</v>
       </c>
       <c r="C80" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -2290,7 +2290,7 @@
         <v>185</v>
       </c>
       <c r="C81" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
@@ -2301,7 +2301,7 @@
         <v>42</v>
       </c>
       <c r="C82" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -2312,7 +2312,7 @@
         <v>124</v>
       </c>
       <c r="C83" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -2323,7 +2323,7 @@
         <v>116</v>
       </c>
       <c r="C84" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -2334,7 +2334,7 @@
         <v>203</v>
       </c>
       <c r="C85" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -2345,7 +2345,7 @@
         <v>60</v>
       </c>
       <c r="C86" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -2356,7 +2356,7 @@
         <v>214</v>
       </c>
       <c r="C87" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -2367,7 +2367,7 @@
         <v>44</v>
       </c>
       <c r="C88" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -2378,7 +2378,7 @@
         <v>163</v>
       </c>
       <c r="C89" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -2389,7 +2389,7 @@
         <v>22</v>
       </c>
       <c r="C90" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -2400,7 +2400,7 @@
         <v>165</v>
       </c>
       <c r="C91" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -2411,7 +2411,7 @@
         <v>40</v>
       </c>
       <c r="C92" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -2433,7 +2433,7 @@
         <v>104</v>
       </c>
       <c r="C94" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -2444,7 +2444,7 @@
         <v>193</v>
       </c>
       <c r="C95" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -2455,7 +2455,7 @@
         <v>140</v>
       </c>
       <c r="C96" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -2466,7 +2466,7 @@
         <v>159</v>
       </c>
       <c r="C97" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -2477,7 +2477,7 @@
         <v>28</v>
       </c>
       <c r="C98" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -2488,7 +2488,7 @@
         <v>84</v>
       </c>
       <c r="C99" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -2499,7 +2499,7 @@
         <v>14</v>
       </c>
       <c r="C100" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -2510,7 +2510,7 @@
         <v>80</v>
       </c>
       <c r="C101" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -2521,7 +2521,7 @@
         <v>68</v>
       </c>
       <c r="C102" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -2532,7 +2532,7 @@
         <v>78</v>
       </c>
       <c r="C103" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -2543,7 +2543,7 @@
         <v>183</v>
       </c>
       <c r="C104" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -2554,7 +2554,7 @@
         <v>72</v>
       </c>
       <c r="C105" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -2565,7 +2565,7 @@
         <v>58</v>
       </c>
       <c r="C106" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -2576,7 +2576,7 @@
         <v>195</v>
       </c>
       <c r="C107" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -2587,73 +2587,73 @@
         <v>211</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
+        <v>322</v>
+      </c>
+      <c r="B109" t="s">
         <v>323</v>
       </c>
-      <c r="B109" t="s">
+      <c r="C109" s="2" t="s">
         <v>324</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
+        <v>325</v>
+      </c>
+      <c r="B110" t="s">
         <v>326</v>
       </c>
-      <c r="B110" t="s">
-        <v>327</v>
-      </c>
       <c r="C110" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
+        <v>327</v>
+      </c>
+      <c r="B111" t="s">
         <v>328</v>
       </c>
-      <c r="B111" t="s">
-        <v>329</v>
-      </c>
       <c r="C111" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
+        <v>329</v>
+      </c>
+      <c r="B112" t="s">
         <v>330</v>
       </c>
-      <c r="B112" t="s">
-        <v>331</v>
-      </c>
       <c r="C112" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
+        <v>331</v>
+      </c>
+      <c r="B113" t="s">
         <v>332</v>
       </c>
-      <c r="B113" t="s">
-        <v>333</v>
-      </c>
       <c r="C113" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
+        <v>337</v>
+      </c>
+      <c r="B114" t="s">
         <v>338</v>
       </c>
-      <c r="B114" t="s">
+      <c r="C114" s="2" t="s">
         <v>339</v>
-      </c>
-      <c r="C114" s="2" t="s">
-        <v>340</v>
       </c>
     </row>
   </sheetData>

</xml_diff>